<commit_message>
augmented the pt graphs
</commit_message>
<xml_diff>
--- a/experiments/compression/results.2017/Fandisk.xlsx
+++ b/experiments/compression/results.2017/Fandisk.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\Documents\plane tree experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\Documents\GitHub\phdThesis\experiments\compression\results.2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="22995" windowHeight="9405" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="270" windowWidth="22995" windowHeight="9405" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -317,11 +317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="500435160"/>
-        <c:axId val="500428888"/>
+        <c:axId val="324042192"/>
+        <c:axId val="324044936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="500435160"/>
+        <c:axId val="324042192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -365,12 +365,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500428888"/>
+        <c:crossAx val="324044936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="500428888"/>
+        <c:axId val="324044936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +408,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500435160"/>
+        <c:crossAx val="324042192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -592,11 +592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="500432416"/>
-        <c:axId val="500430456"/>
+        <c:axId val="324045328"/>
+        <c:axId val="324042584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="500432416"/>
+        <c:axId val="324045328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -635,12 +635,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500430456"/>
+        <c:crossAx val="324042584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="500430456"/>
+        <c:axId val="324042584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +678,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500432416"/>
+        <c:crossAx val="324045328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,11 +847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="500429672"/>
-        <c:axId val="500430064"/>
+        <c:axId val="324043368"/>
+        <c:axId val="363521336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="500429672"/>
+        <c:axId val="324043368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,12 +894,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500430064"/>
+        <c:crossAx val="363521336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="500430064"/>
+        <c:axId val="363521336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +937,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500429672"/>
+        <c:crossAx val="324043368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1121,11 +1121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="500432024"/>
-        <c:axId val="500433592"/>
+        <c:axId val="363514280"/>
+        <c:axId val="363519376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="500432024"/>
+        <c:axId val="363514280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1164,12 +1164,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500433592"/>
+        <c:crossAx val="363519376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="500433592"/>
+        <c:axId val="363519376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -1213,7 +1213,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="500432024"/>
+        <c:crossAx val="363514280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1574,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499710192"/>
-        <c:axId val="499708624"/>
+        <c:axId val="363516240"/>
+        <c:axId val="363520160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499710192"/>
+        <c:axId val="363516240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1623,12 +1623,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499708624"/>
+        <c:crossAx val="363520160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499708624"/>
+        <c:axId val="363520160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -1669,7 +1669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499710192"/>
+        <c:crossAx val="363516240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1751,13 +1751,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1203088803088803</c:v>
+                  <c:v>0.96247104247104243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41822393822393822</c:v>
+                  <c:v>3.3457915057915057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88648648648648654</c:v>
+                  <c:v>7.0918918918918923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2006,11 +2006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499710976"/>
-        <c:axId val="499712544"/>
+        <c:axId val="363516632"/>
+        <c:axId val="363520552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499710976"/>
+        <c:axId val="363516632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2033,18 +2033,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499712544"/>
+        <c:crossAx val="363520552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499712544"/>
+        <c:axId val="363520552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -2067,19 +2068,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499710976"/>
+        <c:crossAx val="363516632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2124,6 +2127,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2153,13 +2157,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.1203088803088803</c:v>
+                  <c:v>0.96247104247104243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41822393822393822</c:v>
+                  <c:v>3.3457915057915057</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88648648648648654</c:v>
+                  <c:v>7.0918918918918923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2338,11 +2342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499707056"/>
-        <c:axId val="499705880"/>
+        <c:axId val="363518200"/>
+        <c:axId val="326209848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499707056"/>
+        <c:axId val="363518200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2365,18 +2369,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499705880"/>
+        <c:crossAx val="326209848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499705880"/>
+        <c:axId val="326209848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2404,19 +2409,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499707056"/>
+        <c:crossAx val="363518200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2675,11 +2682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499706664"/>
-        <c:axId val="509233080"/>
+        <c:axId val="326211024"/>
+        <c:axId val="326211808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499706664"/>
+        <c:axId val="326211024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2702,18 +2709,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509233080"/>
+        <c:crossAx val="326211808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="509233080"/>
+        <c:axId val="326211808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -2736,19 +2744,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499706664"/>
+        <c:crossAx val="326211024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3007,11 +3017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="509235432"/>
-        <c:axId val="509230728"/>
+        <c:axId val="326210240"/>
+        <c:axId val="326215336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="509235432"/>
+        <c:axId val="326210240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3039,18 +3049,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509230728"/>
+        <c:crossAx val="326215336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="509230728"/>
+        <c:axId val="326215336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -3073,19 +3084,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509235432"/>
+        <c:crossAx val="326210240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3157,7 +3170,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -3277,7 +3290,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9172705" cy="6289110"/>
+    <xdr:ext cx="9485856" cy="6289110"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3722,8 +3735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,8 +4023,8 @@
         <v>2.2900000000000001E-4</v>
       </c>
       <c r="I20">
-        <f>(1*E20)/$B$2</f>
-        <v>0.1203088803088803</v>
+        <f>(8*E20)/$B$2</f>
+        <v>0.96247104247104243</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4040,8 +4053,8 @@
         <v>3.3000000000000003E-5</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I22" si="0">(1*E21)/$B$2</f>
-        <v>0.41822393822393822</v>
+        <f>(8*E21)/$B$2</f>
+        <v>3.3457915057915057</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -4070,8 +4083,8 @@
         <v>1.9000000000000001E-5</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0.88648648648648654</v>
+        <f>(8*E22)/$B$2</f>
+        <v>7.0918918918918923</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -4125,7 +4138,7 @@
         <v>1.8799999999999999E-4</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="G27:G34" si="1">(8*C27)/$B$2</f>
+        <f t="shared" ref="G27:G34" si="0">(8*C27)/$B$2</f>
         <v>0.11737451737451737</v>
       </c>
     </row>
@@ -4149,7 +4162,7 @@
         <v>6.3E-5</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.2050965250965251</v>
       </c>
     </row>
@@ -4173,7 +4186,7 @@
         <v>1.7E-5</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.67830115830115834</v>
       </c>
     </row>
@@ -4197,7 +4210,7 @@
         <v>1.5E-5</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.76972972972972975</v>
       </c>
     </row>
@@ -4221,7 +4234,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6345945945945946</v>
       </c>
     </row>
@@ -4245,7 +4258,7 @@
         <v>6.9999999999999999E-6</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6345945945945946</v>
       </c>
     </row>
@@ -4269,7 +4282,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.4568339768339769</v>
       </c>
     </row>
@@ -4293,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27.802934362934362</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-did fandisk and horse
</commit_message>
<xml_diff>
--- a/experiments/compression/results.2017/Fandisk.xlsx
+++ b/experiments/compression/results.2017/Fandisk.xlsx
@@ -17,9 +17,10 @@
     <sheet name="Chart3" sheetId="6" r:id="rId3"/>
     <sheet name="Chart4" sheetId="7" r:id="rId4"/>
     <sheet name="Chart5" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
+    <sheet name="ChartX" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -69,9 +70,6 @@
     <t>MD</t>
   </si>
   <si>
-    <t>khoda</t>
-  </si>
-  <si>
     <t>rms</t>
   </si>
   <si>
@@ -79,9 +77,6 @@
   </si>
   <si>
     <t>rms-4</t>
-  </si>
-  <si>
-    <t>BIO-Tree 14</t>
   </si>
   <si>
     <t xml:space="preserve"> threshold</t>
@@ -124,6 +119,12 @@
   </si>
   <si>
     <t>mse</t>
+  </si>
+  <si>
+    <t>Khodakovsky et al.</t>
+  </si>
+  <si>
+    <t>SOT</t>
   </si>
 </sst>
 </file>
@@ -317,11 +318,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324042192"/>
-        <c:axId val="324044936"/>
+        <c:axId val="324222616"/>
+        <c:axId val="324221832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324042192"/>
+        <c:axId val="324222616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -365,12 +366,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324044936"/>
+        <c:crossAx val="324221832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324044936"/>
+        <c:axId val="324221832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -408,7 +409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324042192"/>
+        <c:crossAx val="324222616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -422,6 +423,738 @@
       <a:noFill/>
     </a:ln>
   </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bayazit et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4102553078054192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6166341333379195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4077529645458378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1988717957537558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1519636085337641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.83675434900379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.6466161991119917E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666945700453262E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.615598098439874E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0366329284376974E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3576982680592147E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6747821879641017E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Khodakovsky et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.2000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plane-Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$27:$G$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11737451737451737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2050965250965251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67830115830115834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76972972972972975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4568339768339769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.802934362934362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3723000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9179999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.176E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8149999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.059E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2799999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="326408184"/>
+        <c:axId val="326412496"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="326408184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Bitrate</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (BPV)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="326412496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="326412496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5000000000000003E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>RMS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="326408184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SOT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$20:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.96247104247104243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3457915057915057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0918918918918923</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$20:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.5134E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7359999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3779999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bayazit et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4102553078054192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6166341333379195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4077529645458378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1988717957537558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1519636085337641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.83675434900379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.6466161991119917E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666945700453262E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.615598098439874E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0366329284376974E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3576982680592147E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6747821879641017E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Khodakovsky et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.2000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plane-Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$27:$G$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11737451737451737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2050965250965251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67830115830115834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76972972972972975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4568339768339769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.802934362934362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3723000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9179999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.176E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8149999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.059E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2799999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="152484416"/>
+        <c:axId val="152492256"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="152484416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Bitrate (bpv)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152492256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="152492256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5000000000000003E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>RMS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152484416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -592,11 +1325,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324045328"/>
-        <c:axId val="324042584"/>
+        <c:axId val="324220264"/>
+        <c:axId val="324220656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324045328"/>
+        <c:axId val="324220264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -635,12 +1368,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324042584"/>
+        <c:crossAx val="324220656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324042584"/>
+        <c:axId val="324220656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -678,7 +1411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324045328"/>
+        <c:crossAx val="324220264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -847,11 +1580,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324043368"/>
-        <c:axId val="363521336"/>
+        <c:axId val="324225360"/>
+        <c:axId val="324226144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324043368"/>
+        <c:axId val="324225360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,12 +1627,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363521336"/>
+        <c:crossAx val="324226144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363521336"/>
+        <c:axId val="324226144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +1670,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324043368"/>
+        <c:crossAx val="324225360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1121,11 +1854,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363514280"/>
-        <c:axId val="363519376"/>
+        <c:axId val="326408968"/>
+        <c:axId val="326407400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363514280"/>
+        <c:axId val="326408968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1164,12 +1897,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363519376"/>
+        <c:crossAx val="326407400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363519376"/>
+        <c:axId val="326407400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -1213,7 +1946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363514280"/>
+        <c:crossAx val="326408968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1380,7 +2113,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>khoda</c:v>
+                  <c:v>Khodakovsky et al.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1574,11 +2307,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363516240"/>
-        <c:axId val="363520160"/>
+        <c:axId val="326410536"/>
+        <c:axId val="326412888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363516240"/>
+        <c:axId val="326410536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1623,12 +2356,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363520160"/>
+        <c:crossAx val="326412888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363520160"/>
+        <c:axId val="326412888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -1669,7 +2402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="363516240"/>
+        <c:crossAx val="326410536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1739,11 +2472,38 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BIO-Tree 14</c:v>
+                  <c:v>SOT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$I$20:$I$22</c:f>
@@ -1796,6 +2556,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$10:$B$15</c:f>
@@ -1861,11 +2648,38 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>khoda</c:v>
+                  <c:v>Khodakovsky et al.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$E$10:$E$14</c:f>
@@ -1930,6 +2744,29 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="50800">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="11"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$G$27:$G$34</c:f>
@@ -2006,11 +2843,437 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363516632"/>
-        <c:axId val="363520552"/>
+        <c:axId val="362878088"/>
+        <c:axId val="362882008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363516632"/>
+        <c:axId val="362878088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="4000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="4000"/>
+                  <a:t>Bitrate (bpv)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362882008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="362882008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.4000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="4000"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU" sz="4000"/>
+                  <a:t>RMS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362878088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41209651047717388"/>
+          <c:y val="5.5500280038216967E-3"/>
+          <c:w val="0.58380512886708846"/>
+          <c:h val="0.48053174315553654"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SOT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$20:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.96247104247104243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3457915057915057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0918918918918923</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$20:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.5134E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7359999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3779999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bayazit et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4102553078054192</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6166341333379195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4077529645458378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1988717957537558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1519636085337641</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.83675434900379</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$10:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.6466161991119917E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1666945700453262E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.615598098439874E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0366329284376974E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3576982680592147E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6747821879641017E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Khodakovsky et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$10:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$10:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.2000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1900000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Plane-Tree</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$27:$G$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.11737451737451737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2050965250965251</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67830115830115834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76972972972972975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6345945945945946</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4568339768339769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.802934362934362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3723000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.9179999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.176E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8149999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6589999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.059E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2799999999999998E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="326408576"/>
+        <c:axId val="326409360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="326408576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2040,12 +3303,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="363520552"/>
+        <c:crossAx val="326409360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="363520552"/>
+        <c:axId val="326409360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -2075,7 +3338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="363516632"/>
+        <c:crossAx val="326408576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2097,7 +3360,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2145,7 +3408,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BIO-Tree 14</c:v>
+                  <c:v>SOT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2197,7 +3460,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>khoda</c:v>
+                  <c:v>Khodakovsky et al.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2342,11 +3605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="363518200"/>
-        <c:axId val="326209848"/>
+        <c:axId val="326413672"/>
+        <c:axId val="326411320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="363518200"/>
+        <c:axId val="326413672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -2376,12 +3639,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326209848"/>
+        <c:crossAx val="326411320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326209848"/>
+        <c:axId val="326411320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,342 +3679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="363518200"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="1"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Bayazit et al.</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$10:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.4102553078054192</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.6166341333379195</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.4077529645458378</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.1988717957537558</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.1519636085337641</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23.83675434900379</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$10:$A$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.6466161991119917E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.1666945700453262E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.615598098439874E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0366329284376974E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.3576982680592147E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6747821879641017E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>khoda</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$10:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$10:$F$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.2000000000000006E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1900000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.0000000000000002E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$25</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plane-Tree</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$27:$G$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0.11737451737451737</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2050965250965251</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.67830115830115834</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.76972972972972975</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6345945945945946</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6345945945945946</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.4568339768339769</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>27.802934362934362</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$27:$E$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1.3723000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.9179999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.176E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8149999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6589999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6589999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.059E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.2799999999999998E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="326211024"/>
-        <c:axId val="326211808"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="326211024"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="25"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Bitrate (bpv)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326211808"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="326211808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.5000000000000003E-2"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Root Mean Square Error</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326211024"/>
+        <c:crossAx val="326413672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2872,7 +3800,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>khoda</c:v>
+                  <c:v>Khodakovsky et al.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3017,11 +3945,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326210240"/>
-        <c:axId val="326215336"/>
+        <c:axId val="326414064"/>
+        <c:axId val="326412104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326210240"/>
+        <c:axId val="326414064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3039,13 +3967,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Bitrate</a:t>
+                  <a:t>Bitrate (bpv)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> (BPV)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3056,12 +3979,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326215336"/>
+        <c:crossAx val="326412104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326215336"/>
+        <c:axId val="326412104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -3079,7 +4002,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>RMS</a:t>
+                  <a:t>Root Mean Square Error</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3091,7 +4014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326210240"/>
+        <c:crossAx val="326414064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3105,11 +4028,6 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3175,6 +4093,17 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -3315,6 +4244,33 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9296400" cy="6070600"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -3381,16 +4337,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3438,6 +4394,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3735,8 +4723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3820,7 +4808,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <f>POWER(10, -4)</f>
@@ -3835,13 +4823,13 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3965,36 +4953,36 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>16</v>
       </c>
-      <c r="G19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" t="s">
-        <v>18</v>
-      </c>
       <c r="I19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -4092,30 +5080,30 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>21</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
         <v>22</v>
       </c>
-      <c r="D26" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="G26" t="s">
         <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished re-doing the pt-sota graphs
</commit_message>
<xml_diff>
--- a/experiments/compression/results.2017/Fandisk.xlsx
+++ b/experiments/compression/results.2017/Fandisk.xlsx
@@ -318,11 +318,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324222616"/>
-        <c:axId val="324221832"/>
+        <c:axId val="321071888"/>
+        <c:axId val="321076984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324222616"/>
+        <c:axId val="321071888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="15"/>
@@ -366,12 +366,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324221832"/>
+        <c:crossAx val="321076984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324221832"/>
+        <c:axId val="321076984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -409,7 +409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324222616"/>
+        <c:crossAx val="321071888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -670,11 +670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326408184"/>
-        <c:axId val="326412496"/>
+        <c:axId val="323230096"/>
+        <c:axId val="323233624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326408184"/>
+        <c:axId val="323230096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -702,19 +702,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326412496"/>
+        <c:crossAx val="323233624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326412496"/>
+        <c:axId val="323233624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -737,21 +736,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326408184"/>
+        <c:crossAx val="323230096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1067,11 +1064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="152484416"/>
-        <c:axId val="152492256"/>
+        <c:axId val="350067856"/>
+        <c:axId val="350061192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152484416"/>
+        <c:axId val="350067856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1094,19 +1091,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152492256"/>
+        <c:crossAx val="350061192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="152492256"/>
+        <c:axId val="350061192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -1129,21 +1125,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152484416"/>
+        <c:crossAx val="350067856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1325,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324220264"/>
-        <c:axId val="324220656"/>
+        <c:axId val="321078160"/>
+        <c:axId val="321077376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324220264"/>
+        <c:axId val="321078160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1368,12 +1362,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324220656"/>
+        <c:crossAx val="321077376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324220656"/>
+        <c:axId val="321077376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1405,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324220264"/>
+        <c:crossAx val="321078160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1580,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="324225360"/>
-        <c:axId val="324226144"/>
+        <c:axId val="321075416"/>
+        <c:axId val="321075808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="324225360"/>
+        <c:axId val="321075416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,12 +1621,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324226144"/>
+        <c:crossAx val="321075808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="324226144"/>
+        <c:axId val="321075808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324225360"/>
+        <c:crossAx val="321075416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1854,11 +1848,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326408968"/>
-        <c:axId val="326407400"/>
+        <c:axId val="321078944"/>
+        <c:axId val="323231664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326408968"/>
+        <c:axId val="321078944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -1897,12 +1891,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326407400"/>
+        <c:crossAx val="323231664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326407400"/>
+        <c:axId val="323231664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
@@ -1946,7 +1940,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326408968"/>
+        <c:crossAx val="321078944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2307,11 +2301,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326410536"/>
-        <c:axId val="326412888"/>
+        <c:axId val="323232448"/>
+        <c:axId val="323229704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326410536"/>
+        <c:axId val="323232448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2339,7 +2333,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2356,12 +2349,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326412888"/>
+        <c:crossAx val="323229704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326412888"/>
+        <c:axId val="323229704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -2385,7 +2378,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2402,7 +2394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326410536"/>
+        <c:crossAx val="323232448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2843,11 +2835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="362878088"/>
-        <c:axId val="362882008"/>
+        <c:axId val="323234016"/>
+        <c:axId val="323237152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="362878088"/>
+        <c:axId val="323234016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -2861,11 +2853,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="4000"/>
+                  <a:defRPr sz="4000" b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU" sz="4000"/>
-                  <a:t>Bitrate (bpv)</a:t>
+                  <a:rPr lang="en-AU" sz="4000" b="0"/>
+                  <a:t>Bit-rate (BPV)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2887,12 +2879,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362882008"/>
+        <c:crossAx val="323237152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="362882008"/>
+        <c:axId val="323237152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.4000000000000002E-2"/>
@@ -2906,10 +2898,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="4000"/>
+                  <a:defRPr sz="4000" b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-AU" sz="4000"/>
+                  <a:rPr lang="en-AU" sz="4000" b="0"/>
                   <a:t>RMS</a:t>
                 </a:r>
               </a:p>
@@ -2932,7 +2924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="362878088"/>
+        <c:crossAx val="323234016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3269,11 +3261,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326408576"/>
-        <c:axId val="326409360"/>
+        <c:axId val="323230880"/>
+        <c:axId val="323232056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326408576"/>
+        <c:axId val="323230880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3296,19 +3288,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326409360"/>
+        <c:crossAx val="323232056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326409360"/>
+        <c:axId val="323232056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -3331,21 +3322,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326408576"/>
+        <c:crossAx val="323230880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3390,7 +3379,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3605,11 +3593,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326413672"/>
-        <c:axId val="326411320"/>
+        <c:axId val="323230488"/>
+        <c:axId val="323235976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326413672"/>
+        <c:axId val="323230488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -3632,19 +3620,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326411320"/>
+        <c:crossAx val="323235976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326411320"/>
+        <c:axId val="323235976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3672,21 +3659,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326413672"/>
+        <c:crossAx val="323230488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3945,11 +3930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="326414064"/>
-        <c:axId val="326412104"/>
+        <c:axId val="323233232"/>
+        <c:axId val="323231272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="326414064"/>
+        <c:axId val="323233232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3972,19 +3957,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326412104"/>
+        <c:crossAx val="323231272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="326412104"/>
+        <c:axId val="323231272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5000000000000003E-2"/>
@@ -4007,21 +3991,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="326414064"/>
+        <c:crossAx val="323233232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4103,7 +4085,8 @@
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 

</xml_diff>